<commit_message>
feat: update README and requirements for enhanced data retrieval and processing features
</commit_message>
<xml_diff>
--- a/mzzb.xlsx
+++ b/mzzb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\mzzbscore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AFF47A-D478-4ADE-BEA0-25E10B320CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA57E4F4-2368-48D8-AE2B-25D5567A3556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3195" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="本季" sheetId="1" r:id="rId1"/>
@@ -76,6 +76,9 @@
     <t>Bangumi</t>
   </si>
   <si>
+    <t>Bangumi_total</t>
+  </si>
+  <si>
     <t>Anilist</t>
   </si>
   <si>
@@ -113,10 +116,6 @@
   </si>
   <si>
     <t>Filmarks_url</t>
-  </si>
-  <si>
-    <t>Bangumi_total</t>
-    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -215,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="65"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,7 +382,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -588,10 +593,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -616,6 +617,16 @@
     <xf numFmtId="49" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -898,7 +909,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -924,19 +935,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:911" ht="30" customHeight="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
     </row>
     <row r="2" spans="1:911" s="18" customFormat="1" ht="36" customHeight="1">
       <c r="A2" s="3" t="s">
@@ -949,46 +960,46 @@
         <v>3</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="17"/>
@@ -1885,8 +1896,8 @@
       <c r="AHZ2" s="17"/>
     </row>
     <row r="3" spans="1:911" ht="36" customHeight="1">
-      <c r="A3" s="74"/>
-      <c r="B3" s="74"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
       <c r="E3" s="27"/>
@@ -1896,13 +1907,8 @@
       <c r="I3" s="27"/>
       <c r="J3" s="30"/>
       <c r="K3" s="30"/>
-      <c r="L3" s="6">
-        <f>C3*0.5+E3*0.2+G3*0.1+J3*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="45">
-        <v>1</v>
-      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="45"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -1910,8 +1916,8 @@
       <c r="R3"/>
     </row>
     <row r="4" spans="1:911" ht="36" customHeight="1">
-      <c r="A4" s="74"/>
-      <c r="B4" s="74"/>
+      <c r="A4" s="80"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="35"/>
       <c r="D4" s="35"/>
       <c r="E4" s="27"/>
@@ -1932,8 +1938,8 @@
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="1:911" ht="36" customHeight="1">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="73"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
       <c r="E5" s="12"/>
@@ -1952,8 +1958,8 @@
       <c r="R5"/>
     </row>
     <row r="6" spans="1:911" ht="36" customHeight="1">
-      <c r="A6" s="75"/>
-      <c r="B6" s="75"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="34"/>
       <c r="D6" s="27"/>
       <c r="E6" s="35"/>
@@ -1972,8 +1978,8 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:911" ht="36" customHeight="1">
-      <c r="A7" s="74"/>
-      <c r="B7" s="74"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="35"/>
       <c r="D7" s="27"/>
       <c r="E7" s="35"/>
@@ -2884,8 +2890,8 @@
       <c r="AHZ7" s="7"/>
     </row>
     <row r="8" spans="1:911" ht="36" customHeight="1">
-      <c r="A8" s="75"/>
-      <c r="B8" s="75"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
       <c r="E8" s="27"/>
@@ -2904,8 +2910,8 @@
       <c r="R8"/>
     </row>
     <row r="9" spans="1:911" s="19" customFormat="1" ht="36" customHeight="1">
-      <c r="A9" s="74"/>
-      <c r="B9" s="74"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
       <c r="E9" s="27"/>
@@ -3817,8 +3823,8 @@
       <c r="AIA9"/>
     </row>
     <row r="10" spans="1:911" ht="36" customHeight="1">
-      <c r="A10" s="75"/>
-      <c r="B10" s="75"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="73"/>
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
       <c r="E10" s="27"/>
@@ -4729,8 +4735,8 @@
       <c r="AHZ10" s="7"/>
     </row>
     <row r="11" spans="1:911" s="19" customFormat="1" ht="36" customHeight="1">
-      <c r="A11" s="75"/>
-      <c r="B11" s="76"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
       <c r="E11" s="27"/>
@@ -5642,8 +5648,8 @@
       <c r="AIA11"/>
     </row>
     <row r="12" spans="1:911" ht="36" customHeight="1">
-      <c r="A12" s="74"/>
-      <c r="B12" s="77"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
       <c r="E12" s="27"/>
@@ -6554,8 +6560,8 @@
       <c r="AHZ12" s="7"/>
     </row>
     <row r="13" spans="1:911" ht="36" customHeight="1">
-      <c r="A13" s="78"/>
-      <c r="B13" s="77"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
       <c r="E13" s="27"/>
@@ -6574,8 +6580,8 @@
       <c r="R13"/>
     </row>
     <row r="14" spans="1:911" ht="36" customHeight="1">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="34"/>
       <c r="D14" s="34"/>
       <c r="E14" s="28"/>
@@ -6594,8 +6600,8 @@
       <c r="R14"/>
     </row>
     <row r="15" spans="1:911" ht="36" customHeight="1">
-      <c r="A15" s="79"/>
-      <c r="B15" s="79"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
       <c r="E15" s="27"/>
@@ -6614,8 +6620,8 @@
       <c r="R15"/>
     </row>
     <row r="16" spans="1:911" ht="36" customHeight="1">
-      <c r="A16" s="75"/>
-      <c r="B16" s="77"/>
+      <c r="A16" s="73"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
       <c r="E16" s="27"/>
@@ -7526,8 +7532,8 @@
       <c r="AHZ16" s="7"/>
     </row>
     <row r="17" spans="1:910" ht="36" customHeight="1">
-      <c r="A17" s="75"/>
-      <c r="B17" s="74"/>
+      <c r="A17" s="73"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="35"/>
       <c r="D17" s="35"/>
       <c r="E17" s="27"/>
@@ -7546,8 +7552,8 @@
       <c r="R17"/>
     </row>
     <row r="18" spans="1:910" ht="36" customHeight="1">
-      <c r="A18" s="79"/>
-      <c r="B18" s="78"/>
+      <c r="A18" s="77"/>
+      <c r="B18" s="76"/>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
       <c r="E18" s="27"/>
@@ -8458,8 +8464,8 @@
       <c r="AHZ18" s="7"/>
     </row>
     <row r="19" spans="1:910" ht="36" customHeight="1">
-      <c r="A19" s="78"/>
-      <c r="B19" s="78"/>
+      <c r="A19" s="76"/>
+      <c r="B19" s="76"/>
       <c r="C19" s="35"/>
       <c r="D19" s="35"/>
       <c r="E19" s="27"/>
@@ -8478,8 +8484,8 @@
       <c r="R19"/>
     </row>
     <row r="20" spans="1:910" ht="36" customHeight="1">
-      <c r="A20" s="74"/>
-      <c r="B20" s="74"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
       <c r="E20" s="27"/>
@@ -9390,8 +9396,8 @@
       <c r="AHZ20" s="7"/>
     </row>
     <row r="21" spans="1:910" ht="36" customHeight="1">
-      <c r="A21" s="75"/>
-      <c r="B21" s="76"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="35"/>
       <c r="D21" s="35"/>
       <c r="E21" s="27"/>
@@ -9410,8 +9416,8 @@
       <c r="R21"/>
     </row>
     <row r="22" spans="1:910" ht="36" customHeight="1">
-      <c r="A22" s="74"/>
-      <c r="B22" s="74"/>
+      <c r="A22" s="72"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
       <c r="E22" s="27"/>
@@ -10322,8 +10328,8 @@
       <c r="AHZ22" s="7"/>
     </row>
     <row r="23" spans="1:910" ht="36" customHeight="1">
-      <c r="A23" s="74"/>
-      <c r="B23" s="75"/>
+      <c r="A23" s="72"/>
+      <c r="B23" s="73"/>
       <c r="C23" s="35"/>
       <c r="D23" s="35"/>
       <c r="E23" s="27"/>
@@ -11234,8 +11240,8 @@
       <c r="AHZ23" s="7"/>
     </row>
     <row r="24" spans="1:910" ht="36" customHeight="1">
-      <c r="A24" s="75"/>
-      <c r="B24" s="75"/>
+      <c r="A24" s="73"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="35"/>
       <c r="D24" s="35"/>
       <c r="E24" s="27"/>
@@ -11254,8 +11260,8 @@
       <c r="R24"/>
     </row>
     <row r="25" spans="1:910" ht="36" customHeight="1">
-      <c r="A25" s="75"/>
-      <c r="B25" s="74"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="72"/>
       <c r="C25" s="34"/>
       <c r="D25" s="34"/>
       <c r="E25" s="27"/>
@@ -12166,8 +12172,8 @@
       <c r="AHZ25" s="7"/>
     </row>
     <row r="26" spans="1:910" ht="36" customHeight="1">
-      <c r="A26" s="75"/>
-      <c r="B26" s="75"/>
+      <c r="A26" s="73"/>
+      <c r="B26" s="73"/>
       <c r="C26" s="35"/>
       <c r="D26" s="35"/>
       <c r="E26" s="27"/>
@@ -12186,8 +12192,8 @@
       <c r="R26"/>
     </row>
     <row r="27" spans="1:910" ht="36" customHeight="1">
-      <c r="A27" s="75"/>
-      <c r="B27" s="75"/>
+      <c r="A27" s="73"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="34"/>
       <c r="D27" s="34"/>
       <c r="E27" s="27"/>
@@ -13098,8 +13104,8 @@
       <c r="AHZ27" s="7"/>
     </row>
     <row r="28" spans="1:910" ht="36" customHeight="1">
-      <c r="A28" s="75"/>
-      <c r="B28" s="80"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="78"/>
       <c r="C28" s="35"/>
       <c r="D28" s="35"/>
       <c r="E28" s="27"/>
@@ -14010,8 +14016,8 @@
       <c r="AHZ28" s="7"/>
     </row>
     <row r="29" spans="1:910" ht="36" customHeight="1">
-      <c r="A29" s="74"/>
-      <c r="B29" s="74"/>
+      <c r="A29" s="72"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="35"/>
       <c r="D29" s="35"/>
       <c r="E29" s="28"/>
@@ -14922,8 +14928,8 @@
       <c r="AHZ29" s="7"/>
     </row>
     <row r="30" spans="1:910" ht="36" customHeight="1">
-      <c r="A30" s="79"/>
-      <c r="B30" s="78"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="76"/>
       <c r="C30" s="41"/>
       <c r="D30" s="35"/>
       <c r="E30" s="27"/>
@@ -15834,8 +15840,8 @@
       <c r="AHZ30" s="7"/>
     </row>
     <row r="31" spans="1:910" ht="36" customHeight="1">
-      <c r="A31" s="74"/>
-      <c r="B31" s="74"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="72"/>
       <c r="C31" s="41"/>
       <c r="D31" s="35"/>
       <c r="E31" s="28"/>
@@ -16746,8 +16752,8 @@
       <c r="AHZ31" s="7"/>
     </row>
     <row r="32" spans="1:910" ht="36" customHeight="1">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
+      <c r="A32" s="75"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="41"/>
       <c r="D32" s="35"/>
       <c r="E32" s="27"/>
@@ -17658,8 +17664,8 @@
       <c r="AHZ32" s="7"/>
     </row>
     <row r="33" spans="1:911" ht="36" customHeight="1">
-      <c r="A33" s="75"/>
-      <c r="B33" s="80"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="41"/>
       <c r="D33" s="35"/>
       <c r="E33" s="27"/>
@@ -17678,8 +17684,8 @@
       <c r="R33"/>
     </row>
     <row r="34" spans="1:911" ht="36" customHeight="1">
-      <c r="A34" s="75"/>
-      <c r="B34" s="74"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="72"/>
       <c r="C34" s="42"/>
       <c r="D34" s="34"/>
       <c r="E34" s="26"/>
@@ -18590,8 +18596,8 @@
       <c r="AHZ34" s="7"/>
     </row>
     <row r="35" spans="1:911" ht="36" customHeight="1">
-      <c r="A35" s="75"/>
-      <c r="B35" s="75"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="41"/>
       <c r="D35" s="35"/>
       <c r="E35" s="27"/>
@@ -19502,8 +19508,8 @@
       <c r="AHZ35" s="7"/>
     </row>
     <row r="36" spans="1:911" ht="36" customHeight="1">
-      <c r="A36" s="74"/>
-      <c r="B36" s="74"/>
+      <c r="A36" s="72"/>
+      <c r="B36" s="72"/>
       <c r="C36" s="41"/>
       <c r="D36" s="35"/>
       <c r="E36" s="27"/>
@@ -20414,8 +20420,8 @@
       <c r="AHZ36" s="7"/>
     </row>
     <row r="37" spans="1:911" ht="36" customHeight="1">
-      <c r="A37" s="75"/>
-      <c r="B37" s="75"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="41"/>
       <c r="D37" s="35"/>
       <c r="E37" s="27"/>
@@ -21326,8 +21332,8 @@
       <c r="AHZ37" s="7"/>
     </row>
     <row r="38" spans="1:911" ht="36" customHeight="1">
-      <c r="A38" s="78"/>
-      <c r="B38" s="78"/>
+      <c r="A38" s="76"/>
+      <c r="B38" s="76"/>
       <c r="C38" s="41"/>
       <c r="D38" s="35"/>
       <c r="E38" s="27"/>
@@ -22238,8 +22244,8 @@
       <c r="AHZ38" s="7"/>
     </row>
     <row r="39" spans="1:911" ht="36" customHeight="1">
-      <c r="A39" s="75"/>
-      <c r="B39" s="80"/>
+      <c r="A39" s="73"/>
+      <c r="B39" s="78"/>
       <c r="C39" s="41"/>
       <c r="D39" s="35"/>
       <c r="E39" s="27"/>
@@ -23150,8 +23156,8 @@
       <c r="AHZ39" s="7"/>
     </row>
     <row r="40" spans="1:911" ht="36" customHeight="1">
-      <c r="A40" s="75"/>
-      <c r="B40" s="75"/>
+      <c r="A40" s="73"/>
+      <c r="B40" s="73"/>
       <c r="C40" s="41"/>
       <c r="D40" s="35"/>
       <c r="E40" s="27"/>
@@ -24062,8 +24068,8 @@
       <c r="AHZ40" s="7"/>
     </row>
     <row r="41" spans="1:911" ht="36" customHeight="1">
-      <c r="A41" s="75"/>
-      <c r="B41" s="77"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="75"/>
       <c r="C41" s="35"/>
       <c r="D41" s="35"/>
       <c r="E41" s="27"/>
@@ -24974,8 +24980,8 @@
       <c r="AHZ41" s="7"/>
     </row>
     <row r="42" spans="1:911" ht="36" customHeight="1">
-      <c r="A42" s="79"/>
-      <c r="B42" s="81"/>
+      <c r="A42" s="77"/>
+      <c r="B42" s="79"/>
       <c r="C42" s="35"/>
       <c r="D42" s="35"/>
       <c r="E42" s="28"/>
@@ -25886,8 +25892,8 @@
       <c r="AHZ42" s="7"/>
     </row>
     <row r="43" spans="1:911" ht="36" customHeight="1">
-      <c r="A43" s="75"/>
-      <c r="B43" s="75"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="73"/>
       <c r="C43" s="35"/>
       <c r="D43" s="35"/>
       <c r="E43" s="27"/>
@@ -25906,8 +25912,8 @@
       <c r="R43"/>
     </row>
     <row r="44" spans="1:911" ht="36" customHeight="1">
-      <c r="A44" s="79"/>
-      <c r="B44" s="79"/>
+      <c r="A44" s="77"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="34"/>
       <c r="D44" s="34"/>
       <c r="E44" s="27"/>
@@ -26818,8 +26824,8 @@
       <c r="AHZ44" s="7"/>
     </row>
     <row r="45" spans="1:911" s="19" customFormat="1" ht="36" customHeight="1">
-      <c r="A45" s="75"/>
-      <c r="B45" s="75"/>
+      <c r="A45" s="73"/>
+      <c r="B45" s="73"/>
       <c r="C45" s="35"/>
       <c r="D45" s="35"/>
       <c r="E45" s="27"/>
@@ -27731,8 +27737,8 @@
       <c r="AIA45"/>
     </row>
     <row r="46" spans="1:911" ht="36" customHeight="1">
-      <c r="A46" s="75"/>
-      <c r="B46" s="74"/>
+      <c r="A46" s="73"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="35"/>
       <c r="D46" s="35"/>
       <c r="E46" s="27"/>
@@ -28643,8 +28649,8 @@
       <c r="AHZ46" s="7"/>
     </row>
     <row r="47" spans="1:911" ht="36" customHeight="1">
-      <c r="A47" s="75"/>
-      <c r="B47" s="77"/>
+      <c r="A47" s="73"/>
+      <c r="B47" s="75"/>
       <c r="C47" s="35"/>
       <c r="D47" s="35"/>
       <c r="E47" s="27"/>
@@ -28663,8 +28669,8 @@
       <c r="R47"/>
     </row>
     <row r="48" spans="1:911" ht="36" customHeight="1">
-      <c r="A48" s="78"/>
-      <c r="B48" s="78"/>
+      <c r="A48" s="76"/>
+      <c r="B48" s="76"/>
       <c r="C48" s="34"/>
       <c r="D48" s="34"/>
       <c r="E48" s="28"/>
@@ -28683,8 +28689,8 @@
       <c r="R48"/>
     </row>
     <row r="49" spans="1:911" ht="36" customHeight="1">
-      <c r="A49" s="75"/>
-      <c r="B49" s="77"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="75"/>
       <c r="C49" s="34"/>
       <c r="D49" s="34"/>
       <c r="E49" s="27"/>
@@ -29595,8 +29601,8 @@
       <c r="AHZ49" s="7"/>
     </row>
     <row r="50" spans="1:911" ht="36" customHeight="1">
-      <c r="A50" s="74"/>
-      <c r="B50" s="77"/>
+      <c r="A50" s="72"/>
+      <c r="B50" s="75"/>
       <c r="C50" s="35"/>
       <c r="D50" s="35"/>
       <c r="E50" s="27"/>
@@ -30507,8 +30513,8 @@
       <c r="AHZ50" s="7"/>
     </row>
     <row r="51" spans="1:911" ht="36" customHeight="1">
-      <c r="A51" s="74"/>
-      <c r="B51" s="77"/>
+      <c r="A51" s="72"/>
+      <c r="B51" s="75"/>
       <c r="C51" s="35"/>
       <c r="D51" s="35"/>
       <c r="E51" s="27"/>
@@ -30527,8 +30533,8 @@
       <c r="R51"/>
     </row>
     <row r="52" spans="1:911" ht="36" customHeight="1">
-      <c r="A52" s="75"/>
-      <c r="B52" s="75"/>
+      <c r="A52" s="73"/>
+      <c r="B52" s="73"/>
       <c r="C52" s="34"/>
       <c r="D52" s="34"/>
       <c r="E52" s="27"/>
@@ -35369,7 +35375,7 @@
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>